<commit_message>
Updated test Cases file
</commit_message>
<xml_diff>
--- a/ProjectDocs/Artifacts/Squander Test Cases.xlsx
+++ b/ProjectDocs/Artifacts/Squander Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80d71404950ebe3a/Master CourseWork/CS691-Spring2022-Deliverable/Squander/ProjectDocs/Artifacts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakan\OneDrive\Master CourseWork\CS691-Spring2022-Deliverable\Squander\ProjectDocs\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{41EAF76E-A3DA-42E8-A33A-00D3D44C9F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A5B55B-6CB5-485A-BB4E-B681C03AF6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{6C8D4292-3192-40BA-834E-1225B1314263}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="7" xr2:uid="{6C8D4292-3192-40BA-834E-1225B1314263}"/>
   </bookViews>
   <sheets>
     <sheet name="Home Screen" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Result Screen" sheetId="5" r:id="rId3"/>
     <sheet name="About Us Screen" sheetId="2" r:id="rId4"/>
     <sheet name="Capture Screen" sheetId="3" r:id="rId5"/>
+    <sheet name="Recycling Stats" sheetId="6" r:id="rId6"/>
+    <sheet name="User Feedback" sheetId="7" r:id="rId7"/>
+    <sheet name="Request Pickup Scheduling" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="197">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -409,6 +412,228 @@
   </si>
   <si>
     <t>Once the user is on the Contribution Screen, it will show the total percentage of global impact on the earth due to the amount of waste generated.</t>
+  </si>
+  <si>
+    <t>SQD-76</t>
+  </si>
+  <si>
+    <t>SQD-135</t>
+  </si>
+  <si>
+    <t>Locate the Stats icon on the Nav Bar</t>
+  </si>
+  <si>
+    <t>User should be able to locate the Stats icon on the Nav Bar</t>
+  </si>
+  <si>
+    <t>User is able to locate the Stats icon on the Nav Bar</t>
+  </si>
+  <si>
+    <t>SQD-136</t>
+  </si>
+  <si>
+    <t>Stats of recycle item visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to see the Stats of all the item they have recycled </t>
+  </si>
+  <si>
+    <t>Once the user is on the Stats Screen they are able to see their Stats of recycled items</t>
+  </si>
+  <si>
+    <t>SQD-137</t>
+  </si>
+  <si>
+    <t>Detailed view of Stats with company name, date &amp; item</t>
+  </si>
+  <si>
+    <t>User should be able to see the details of the recycling company they have used to recycle a item along with date</t>
+  </si>
+  <si>
+    <t>Once the user is on the Stats Screen, they are able to see the recycling company name along with the particular  items they have recycled along with the date they have done.</t>
+  </si>
+  <si>
+    <t>Recycling Statistics</t>
+  </si>
+  <si>
+    <t>User Feedback</t>
+  </si>
+  <si>
+    <t>SQD-130</t>
+  </si>
+  <si>
+    <t>Locate the Contact Team Icon on the Nav Bar</t>
+  </si>
+  <si>
+    <t>User should be able to locate the Contact Team icon on the Nav Bar</t>
+  </si>
+  <si>
+    <t>User is able to locate the Contact Team icon on the Nav Bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SQD-131</t>
+  </si>
+  <si>
+    <t>Click on the Contact Team icon</t>
+  </si>
+  <si>
+    <t>User should be able to see the Contact Team icon   on the Nav Bar and it should be clickable</t>
+  </si>
+  <si>
+    <t>Once the user click on the Contact Team icon and its is clickable and taking to a new screen</t>
+  </si>
+  <si>
+    <t>SQD-132</t>
+  </si>
+  <si>
+    <t>Locate Contact team email</t>
+  </si>
+  <si>
+    <t>User should be able to see the Squander Contact Team email address</t>
+  </si>
+  <si>
+    <t>One the user is on the Contact Team screen, they are able to see the email address</t>
+  </si>
+  <si>
+    <t>SQD-133</t>
+  </si>
+  <si>
+    <t>Locate Contact Team Phone Number</t>
+  </si>
+  <si>
+    <t>User should be able to see the Squander Contact Team phone number</t>
+  </si>
+  <si>
+    <t>One the user is on the Contact Team screen, they are able to see the phone number</t>
+  </si>
+  <si>
+    <t>SQD-134</t>
+  </si>
+  <si>
+    <t>Locate Feedback Request Button</t>
+  </si>
+  <si>
+    <t>User should be able to see the User Feedback Request Button</t>
+  </si>
+  <si>
+    <t>Once the user is on the Contact Team Screen, they are able to see the Feedback request button which is clickable</t>
+  </si>
+  <si>
+    <t>Request Pickup Scheduling</t>
+  </si>
+  <si>
+    <t>SQD-73</t>
+  </si>
+  <si>
+    <t>SQD-138</t>
+  </si>
+  <si>
+    <t>Locate the Recycling Company Detail Button</t>
+  </si>
+  <si>
+    <t>User should be able to see the Recycling company Detail Button and it is clickable.</t>
+  </si>
+  <si>
+    <t>Once the user is on the Recycling company list along with the Detail Button which is clickable</t>
+  </si>
+  <si>
+    <t>SQD-139</t>
+  </si>
+  <si>
+    <t>View the Recycling Company Details</t>
+  </si>
+  <si>
+    <t>User should be able to view the details of the recycling company</t>
+  </si>
+  <si>
+    <t>Once the user is on the recycling page and it click on a company it will pop the details of the company.</t>
+  </si>
+  <si>
+    <t>SQD-140</t>
+  </si>
+  <si>
+    <t>Locate the Contact Button</t>
+  </si>
+  <si>
+    <t>User should be able to see the Contact Button and its should be clickable</t>
+  </si>
+  <si>
+    <t>One the user is on the Detail Screen,they can see a contact button and it is clickable</t>
+  </si>
+  <si>
+    <t>SQD-141</t>
+  </si>
+  <si>
+    <t>Locate company address, phone no, &amp; website</t>
+  </si>
+  <si>
+    <t>User should be able to view the recycling company address, phone number &amp; website</t>
+  </si>
+  <si>
+    <t>Once the user is on the Detail Screen, they are able to view the recycling company address, phone no &amp; website</t>
+  </si>
+  <si>
+    <t>SQD-142</t>
+  </si>
+  <si>
+    <t>Click on the Contact Button</t>
+  </si>
+  <si>
+    <t>User should be able to click on the Contact Button and a new Request screen should pop up</t>
+  </si>
+  <si>
+    <t>Once the user click on the Contact Button a new Request Screen open up</t>
+  </si>
+  <si>
+    <t>SQD-143</t>
+  </si>
+  <si>
+    <t>Locate the Request Screen</t>
+  </si>
+  <si>
+    <t>User should be able to see the Request screen with the waste image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One the user clicks on Contact Button a Request screen is visible with waste image </t>
+  </si>
+  <si>
+    <t>SQD-144</t>
+  </si>
+  <si>
+    <t>View Description Text Box</t>
+  </si>
+  <si>
+    <t>User should be able to view the Description text where we can enter our details upto 1000 characters</t>
+  </si>
+  <si>
+    <t>Once the user is on the Request Screen, a Description Text Box is visible and where we can enter upto 1000 characters.</t>
+  </si>
+  <si>
+    <t>SQD-145</t>
+  </si>
+  <si>
+    <t>Locate Request Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to view the Request Button </t>
+  </si>
+  <si>
+    <t>Once the user is on the request screen, a request button is visible</t>
+  </si>
+  <si>
+    <t>SQD146</t>
+  </si>
+  <si>
+    <t>View Request Alert</t>
+  </si>
+  <si>
+    <t>Once the user click on the request button, a request should be sent to the company and an alert should be shown</t>
+  </si>
+  <si>
+    <t>Once the user click on the request button, a request is sent to recycling company and an alert is shown to user stating the same.</t>
   </si>
 </sst>
 </file>
@@ -567,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -608,6 +833,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,8 +900,8 @@
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color rgb="FF7D5F02"/>
         </left>
@@ -646,14 +910,29 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="medium">
-          <color rgb="FF7D5F02"/>
-        </vertical>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="7" tint="-0.499984740745262"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color theme="7" tint="-0.499984740745262"/>
+        </top>
         <bottom style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </bottom>
@@ -672,24 +951,6 @@
         <scheme val="none"/>
       </font>
       <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </vertical>
-        <horizontal style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -715,7 +976,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </left>
@@ -728,12 +989,6 @@
         <bottom style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </bottom>
-        <vertical style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </vertical>
-        <horizontal style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -756,7 +1011,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </left>
@@ -769,12 +1024,6 @@
         <bottom style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </bottom>
-        <vertical style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </vertical>
-        <horizontal style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -797,7 +1046,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </left>
@@ -810,12 +1059,6 @@
         <bottom style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </bottom>
-        <vertical style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </vertical>
-        <horizontal style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -831,7 +1074,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </left>
@@ -844,57 +1088,6 @@
         <bottom style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </bottom>
-        <vertical style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </vertical>
-        <horizontal style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="7" tint="-0.499984740745262"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </left>
-        <right style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </right>
-        <top style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </vertical>
-        <horizontal style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -921,7 +1114,46 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="7" tint="-0.499984740745262"/>
+        </left>
+        <right style="medium">
+          <color theme="7" tint="-0.499984740745262"/>
+        </right>
+        <top style="medium">
+          <color theme="7" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="medium">
+          <color theme="7" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="7" tint="-0.499984740745262"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="medium">
           <color theme="7" tint="-0.499984740745262"/>
@@ -932,12 +1164,6 @@
         <bottom style="medium">
           <color theme="7" tint="-0.499984740745262"/>
         </bottom>
-        <vertical style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </vertical>
-        <horizontal style="medium">
-          <color theme="7" tint="-0.499984740745262"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -964,17 +1190,11 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <name val="Trebuchet MS"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
+      <border>
+        <bottom style="medium">
+          <color theme="7" tint="-0.499984740745262"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -990,7 +1210,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D757B99C-04A3-498C-B7E8-2FB54344928E}" name="Table9131415" displayName="Table9131415" ref="B2:H6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="11" headerRowBorderDxfId="1" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D757B99C-04A3-498C-B7E8-2FB54344928E}" name="Table9131415" displayName="Table9131415" ref="B2:H6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="2" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{76B2CA57-A02E-4738-B5DF-B00CC673B0D9}" name="Test Case Name" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{0157BD1B-3A2D-4ECE-8A7A-A49C0082A381}" name="User Story" dataDxfId="7"/>
@@ -998,7 +1218,7 @@
     <tableColumn id="4" xr3:uid="{B4915873-E4C8-4272-88F9-22771FEC3694}" name="Test Action" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{F5888C3C-3B4D-4F43-9853-1AEDEDD87D42}" name="Expected Results" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{0986ED95-B22D-4B78-997D-82909521274C}" name="Test Result" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{B418DA15-E181-4F1E-8D31-9D799637AE69}" name="Pass/Fail" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{B418DA15-E181-4F1E-8D31-9D799637AE69}" name="Pass/Fail" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1653,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D24EDB1-1E1A-4730-92F4-0D3840C3ECB0}">
   <dimension ref="B1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1664,6 +1884,7 @@
     <col min="5" max="5" width="12.08984375" customWidth="1"/>
     <col min="6" max="6" width="38.1796875" customWidth="1"/>
     <col min="7" max="7" width="42.26953125" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1709,7 +1930,7 @@
       <c r="G3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1728,7 +1949,7 @@
       <c r="G4" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1747,7 +1968,7 @@
       <c r="G5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1766,7 +1987,7 @@
       <c r="G6" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1785,7 +2006,7 @@
       <c r="G7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1799,7 +2020,7 @@
   <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1808,109 +2029,110 @@
     <col min="5" max="5" width="18.90625" customWidth="1"/>
     <col min="6" max="6" width="28.54296875" customWidth="1"/>
     <col min="7" max="7" width="37.1796875" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1926,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885B4B97-CF54-4E34-83D2-1FD75E61CF9A}">
   <dimension ref="B1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1965,139 +2187,639 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD13A2D0-BDF4-41C9-9B41-94731E0FF17A}">
+  <dimension ref="B1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="13.90625" customWidth="1"/>
+    <col min="6" max="6" width="38" customWidth="1"/>
+    <col min="7" max="7" width="45.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.08984375" style="17" customWidth="1"/>
+    <col min="9" max="9" width="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35117E46-4113-4C43-A95C-5B6C7FD1009E}">
+  <dimension ref="B1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
+    <col min="6" max="6" width="34.81640625" customWidth="1"/>
+    <col min="7" max="7" width="34.54296875" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A288C43-E853-4B3B-80D6-063C352FFDB9}">
+  <dimension ref="B1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.7265625" style="17"/>
+    <col min="4" max="4" width="8.7265625" style="15"/>
+    <col min="5" max="5" width="25.26953125" customWidth="1"/>
+    <col min="6" max="6" width="41.26953125" customWidth="1"/>
+    <col min="7" max="7" width="41.36328125" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>